<commit_message>
Added descriptive text to combined_results.xlsx
</commit_message>
<xml_diff>
--- a/data/combined_results.xlsx
+++ b/data/combined_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\workspaces_local\cs598_dl4hc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_598_DLH\Project\cs598_dl4hc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9232C31-9736-48FF-8D0C-1F0A004B14FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778462C7-CF00-41AB-9EA4-8C0D8999AD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9518" yWindow="3900" windowWidth="20385" windowHeight="11873" xr2:uid="{59E9A702-F97F-4DEA-85B4-913AD7B3CD01}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="22305" windowHeight="13995" xr2:uid="{59E9A702-F97F-4DEA-85B4-913AD7B3CD01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Schema</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">Health          </t>
   </si>
   <si>
-    <t xml:space="preserve">Power \&amp; ctrl   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Meta-cognition  </t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Combined Reproduced Results</t>
   </si>
   <si>
-    <t>Kurt Touhy and Michael Miller</t>
-  </si>
-  <si>
     <t>CS598 Deep Learning for Healthcare</t>
   </si>
   <si>
@@ -98,6 +92,15 @@
   </si>
   <si>
     <t>Single LSTM</t>
+  </si>
+  <si>
+    <t>Kurt Tuohy and Michael Miller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power &amp; ctrl   </t>
+  </si>
+  <si>
+    <t>For each model type, displays Spearman rank-order correlation between ground-truth and predicted correspondence of utterances to schemas.</t>
   </si>
 </sst>
 </file>
@@ -173,13 +176,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,47 +498,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051F57C7-9C95-4DEE-9160-691021FC1058}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="7" width="10.73046875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44686</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -543,28 +546,28 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="5"/>
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -587,7 +590,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -610,7 +613,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -633,7 +636,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -656,9 +659,9 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>0.18</v>
@@ -679,18 +682,18 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
         <v>0.02</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4">
         <v>7.0000000000000007E-2</v>
@@ -702,9 +705,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="4">
         <v>-0.01</v>
@@ -725,9 +728,9 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4">
         <v>0.59</v>
@@ -748,9 +751,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4">
         <v>0.42</v>
@@ -769,6 +772,11 @@
       </c>
       <c r="G16" s="2">
         <v>0.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>